<commit_message>
clases de equiv. doc correcciones
</commit_message>
<xml_diff>
--- a/docs/reporte-issues/graficos.xlsx
+++ b/docs/reporte-issues/graficos.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new-obli\proyecto-grupo-4-olivieri-urreta\docs\reporte-issues\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Diego/Desktop/ORT/ingenieria-de-software/proyecto-grupo-4-olivieri-urreta/docs/reporte-issues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A365D4F-5D2A-4280-87C7-B96006269D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D15331-41DF-A84E-95AA-41BA35C30EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja3" sheetId="3" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="Pivot totales" sheetId="3" r:id="rId1"/>
+    <sheet name="Tabla por issue" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Num Issue</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>invalidd</t>
-  </si>
-  <si>
-    <t>wontfixx</t>
   </si>
   <si>
     <t>enhancementt</t>
@@ -61,9 +58,6 @@
     <t>Invalid</t>
   </si>
   <si>
-    <t>Wontfix</t>
-  </si>
-  <si>
     <t>Enhancement</t>
   </si>
   <si>
@@ -74,6 +68,9 @@
   </si>
   <si>
     <t>Accesibilidad</t>
+  </si>
+  <si>
+    <t>wontfix</t>
   </si>
 </sst>
 </file>
@@ -166,7 +163,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -177,7 +174,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[graficos.xlsx]Hoja3!TablaDinámica2</c:name>
+    <c:name>[graficos.xlsx]Pivot totales!TablaDinámica2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -225,7 +222,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-UY"/>
+              <a:endParaRPr lang="en-UY"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -281,7 +278,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-UY"/>
+              <a:endParaRPr lang="en-UY"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -337,7 +334,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-UY"/>
+              <a:endParaRPr lang="en-UY"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -393,7 +390,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-UY"/>
+              <a:endParaRPr lang="en-UY"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -449,7 +446,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-UY"/>
+              <a:endParaRPr lang="en-UY"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -505,7 +502,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-UY"/>
+              <a:endParaRPr lang="en-UY"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -561,7 +558,63 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-UY"/>
+              <a:endParaRPr lang="en-UY"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-UY"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -587,7 +640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$3</c:f>
+              <c:f>'Pivot totales'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -608,7 +661,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -619,12 +672,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -640,7 +693,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$3</c:f>
+              <c:f>'Pivot totales'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -661,7 +714,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -672,12 +725,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$B$4</c:f>
+              <c:f>'Pivot totales'!$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -693,11 +746,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$3</c:f>
+              <c:f>'Pivot totales'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Wontfix</c:v>
+                  <c:v>Enhancement</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -714,7 +767,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -725,12 +778,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$C$4</c:f>
+              <c:f>'Pivot totales'!$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -746,11 +799,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$D$3</c:f>
+              <c:f>'Pivot totales'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Enhancement</c:v>
+                  <c:v>Usabilidad</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -767,7 +820,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -778,12 +831,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$D$4</c:f>
+              <c:f>'Pivot totales'!$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -799,11 +852,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$E$3</c:f>
+              <c:f>'Pivot totales'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Usabilidad</c:v>
+                  <c:v>Documentation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -820,7 +873,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -831,12 +884,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$E$4</c:f>
+              <c:f>'Pivot totales'!$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -852,11 +905,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$F$3</c:f>
+              <c:f>'Pivot totales'!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Documentation</c:v>
+                  <c:v>Accesibilidad</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -873,7 +926,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -884,12 +937,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$F$4</c:f>
+              <c:f>'Pivot totales'!$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,11 +958,11 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$G$3</c:f>
+              <c:f>'Pivot totales'!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Accesibilidad</c:v>
+                  <c:v>wontfix</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -928,7 +981,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja3!$A$4</c:f>
+              <c:f>'Pivot totales'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -939,19 +992,19 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$G$4</c:f>
+              <c:f>'Pivot totales'!$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-F02A-4F79-A167-62C4DA40E602}"/>
+              <c16:uniqueId val="{00000001-A909-1944-B787-EF4DDEA7B3CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1009,7 +1062,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-UY"/>
+            <a:endParaRPr lang="en-UY"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="830117872"/>
@@ -1091,7 +1144,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-UY"/>
+            <a:endParaRPr lang="en-UY"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="830118704"/>
@@ -1121,7 +1174,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1133,7 +1186,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-UY"/>
+          <a:endParaRPr lang="en-UY"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1168,7 +1221,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-UY"/>
+      <a:endParaRPr lang="en-UY"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1741,16 +1794,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>765175</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>96837</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1779,13 +1832,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Giovanni" refreshedDate="44528.203785185186" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="19" xr:uid="{BBD2E0D9-9308-49BE-9374-44FFA5214FE7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Diego" refreshedDate="44528.553779166665" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="23" xr:uid="{BBD2E0D9-9308-49BE-9374-44FFA5214FE7}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabla1"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Num Issue" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="17" maxValue="47"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="17" maxValue="51"/>
     </cacheField>
     <cacheField name="bugg" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
@@ -1793,7 +1846,7 @@
     <cacheField name="invalidd" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
     </cacheField>
-    <cacheField name="wontfixx" numFmtId="0">
+    <cacheField name="wontfix" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
     </cacheField>
     <cacheField name="enhancementt" numFmtId="0">
@@ -1818,7 +1871,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="19">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="23">
   <r>
     <n v="17"/>
     <n v="1"/>
@@ -1831,8 +1884,8 @@
   </r>
   <r>
     <n v="22"/>
-    <n v="1"/>
-    <m/>
+    <m/>
+    <n v="1"/>
     <m/>
     <m/>
     <m/>
@@ -1921,7 +1974,7 @@
   </r>
   <r>
     <n v="39"/>
-    <n v="1"/>
+    <m/>
     <m/>
     <m/>
     <m/>
@@ -1931,7 +1984,7 @@
   </r>
   <r>
     <n v="40"/>
-    <n v="1"/>
+    <m/>
     <m/>
     <m/>
     <m/>
@@ -2008,18 +2061,58 @@
     <m/>
     <m/>
     <n v="1"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="49"/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="50"/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="51"/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0835616F-9B91-4A4A-93FF-580781CCA4DF}" name="TablaDinámica2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0835616F-9B91-4A4A-93FF-580781CCA4DF}" name="TablaDinámica2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A3:G4" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField name="wontfix2" dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -2057,13 +2150,13 @@
   <dataFields count="7">
     <dataField name="Bug" fld="1" baseField="0" baseItem="0"/>
     <dataField name="Invalid" fld="2" baseField="0" baseItem="0"/>
-    <dataField name="Wontfix" fld="3" baseField="0" baseItem="0"/>
     <dataField name="Enhancement" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Usabilidad" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Documentation" fld="6" baseField="0" baseItem="0"/>
     <dataField name="Accesibilidad" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="wontfix" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="21">
+  <chartFormats count="19">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -2082,7 +2175,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
+    <chartFormat chart="0" format="3" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2091,7 +2184,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
+    <chartFormat chart="0" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2100,7 +2193,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
+    <chartFormat chart="0" format="5" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2109,20 +2202,11 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="5" series="1">
+    <chartFormat chart="0" format="6" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -2145,7 +2229,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="1" format="9" series="1">
+    <chartFormat chart="1" format="10" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2154,7 +2238,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="1" format="10" series="1">
+    <chartFormat chart="1" format="11" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2163,7 +2247,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="1" format="11" series="1">
+    <chartFormat chart="1" format="12" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2172,20 +2256,11 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="1" format="12" series="1">
+    <chartFormat chart="1" format="13" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="13" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -2208,7 +2283,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="16" series="1">
+    <chartFormat chart="2" format="17" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2217,7 +2292,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="17" series="1">
+    <chartFormat chart="2" format="18" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2226,7 +2301,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="18" series="1">
+    <chartFormat chart="2" format="19" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2235,7 +2310,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="19" series="1">
+    <chartFormat chart="2" format="20" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2244,7 +2319,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="20" series="1">
+    <chartFormat chart="0" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2267,17 +2342,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB0CF4E3-160C-4FAA-B4A0-6C328850C809}" name="Tabla1" displayName="Tabla1" ref="B2:I21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B2:I21" xr:uid="{DB0CF4E3-160C-4FAA-B4A0-6C328850C809}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB0CF4E3-160C-4FAA-B4A0-6C328850C809}" name="Tabla1" displayName="Tabla1" ref="B2:I25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I25" xr:uid="{DB0CF4E3-160C-4FAA-B4A0-6C328850C809}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7CE03A6C-F6B1-4A63-A172-8E370E4415FE}" name="Num Issue" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{E54F8D28-CB70-43E8-BCFD-BF1B9466C3B6}" name="bugg" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{290B875B-37B7-430D-BDD4-B2B69DA8E7A0}" name="invalidd" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{97262092-9299-4695-9A82-8693D855C043}" name="wontfixx" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{AA8A16E6-726D-4193-BC5B-A147333A37E3}" name="enhancementt" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4505AE34-2387-43E8-938A-4D632AA711D4}" name="usabilidadd" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{582D21C5-C539-4D71-B5BE-20A5E984D92C}" name="documentationn" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{121D40EF-F8EA-48A1-9336-7E5C24193E87}" name="accesibilidadd" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7CE03A6C-F6B1-4A63-A172-8E370E4415FE}" name="Num Issue" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E54F8D28-CB70-43E8-BCFD-BF1B9466C3B6}" name="bugg" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{290B875B-37B7-430D-BDD4-B2B69DA8E7A0}" name="invalidd" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{97262092-9299-4695-9A82-8693D855C043}" name="wontfix" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{AA8A16E6-726D-4193-BC5B-A147333A37E3}" name="enhancementt" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{4505AE34-2387-43E8-938A-4D632AA711D4}" name="usabilidadd" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{582D21C5-C539-4D71-B5BE-20A5E984D92C}" name="documentationn" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{121D40EF-F8EA-48A1-9336-7E5C24193E87}" name="accesibilidadd" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2548,65 +2623,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4269BDCD-B032-4D90-B6D8-2DFA9C030E88}">
   <dimension ref="A3:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2617,25 +2692,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I21"/>
+  <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="B1:I21"/>
+      <selection activeCell="E3" sqref="E3:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2646,26 +2721,26 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>17</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="1">
@@ -2677,25 +2752,23 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>22</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>24</v>
       </c>
-      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1">
         <v>1</v>
@@ -2705,11 +2778,10 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>25</v>
       </c>
-      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
@@ -2719,11 +2791,10 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>30</v>
       </c>
-      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
@@ -2733,11 +2804,10 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>34</v>
       </c>
-      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>1</v>
       </c>
@@ -2747,11 +2817,11 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>35</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" s="1"/>
@@ -2763,11 +2833,11 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>36</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="1"/>
@@ -2777,11 +2847,11 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>37</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" s="1"/>
@@ -2793,11 +2863,11 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>38</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" s="1"/>
@@ -2809,12 +2879,9 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>39</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2825,12 +2892,9 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>40</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2841,11 +2905,10 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>41</v>
       </c>
-      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2857,11 +2920,10 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>42</v>
       </c>
-      <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>1</v>
       </c>
@@ -2873,11 +2935,10 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>43</v>
       </c>
-      <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>1</v>
       </c>
@@ -2889,11 +2950,11 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>44</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" s="1"/>
@@ -2905,11 +2966,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>45</v>
       </c>
-      <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>1</v>
       </c>
@@ -2921,11 +2981,11 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>46</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" s="1"/>
@@ -2937,11 +2997,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>47</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" s="1"/>
@@ -2952,6 +3012,68 @@
       <c r="I21" s="1">
         <v>1</v>
       </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>48</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>49</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>51</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>